<commit_message>
Adding Final Exam info
</commit_message>
<xml_diff>
--- a/Assignments/Labs/Alex/FinalExamSchema.xlsx
+++ b/Assignments/Labs/Alex/FinalExamSchema.xlsx
@@ -8,19 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SQLRepo\de_code_it_4\Assignments\Labs\Alex\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{799EC451-1FA0-4D80-A928-84267C1B50BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D8606CFB-DEB3-4689-9B3D-AC531B0069C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" tabRatio="812" activeTab="1" xr2:uid="{E31112A4-B4B5-40AA-81F5-9CA00A647AC9}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" tabRatio="812" xr2:uid="{E31112A4-B4B5-40AA-81F5-9CA00A647AC9}"/>
   </bookViews>
   <sheets>
-    <sheet name="Summary" sheetId="7" r:id="rId1"/>
-    <sheet name="Data Example" sheetId="8" r:id="rId2"/>
-    <sheet name="Diagram" sheetId="1" r:id="rId3"/>
-    <sheet name="CustomerInfo - Anjali" sheetId="2" r:id="rId4"/>
-    <sheet name="SurveyInfo -  Katie" sheetId="3" r:id="rId5"/>
-    <sheet name="QuestionTable1 - Tim" sheetId="4" r:id="rId6"/>
-    <sheet name="QuestionTable2 - Erika" sheetId="5" r:id="rId7"/>
-    <sheet name="QuestionTable3 - Lyndon" sheetId="6" r:id="rId8"/>
+    <sheet name="Server Information" sheetId="8" r:id="rId1"/>
+    <sheet name="Diagram" sheetId="1" r:id="rId2"/>
+    <sheet name="CustomerInfo - Anjali" sheetId="2" r:id="rId3"/>
+    <sheet name="SurveyInfo -  Katie" sheetId="3" r:id="rId4"/>
+    <sheet name="QuestionTable1 - Tim" sheetId="4" r:id="rId5"/>
+    <sheet name="QuestionTable2 - Erika" sheetId="5" r:id="rId6"/>
+    <sheet name="QuestionTable3 - Lyndon" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="72">
   <si>
     <t>Field</t>
   </si>
@@ -234,54 +233,47 @@
     <t>N</t>
   </si>
   <si>
-    <t>Helen</t>
-  </si>
-  <si>
-    <t>Haysey</t>
-  </si>
-  <si>
-    <t>847 Gerald Way</t>
-  </si>
-  <si>
-    <t>Boise</t>
-  </si>
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>hhaysey0@addtoany.com</t>
-  </si>
-  <si>
-    <t>How did you hear about Code Black?</t>
-  </si>
-  <si>
-    <t>through a friend</t>
-  </si>
-  <si>
-    <t>What subjects should we cover?</t>
-  </si>
-  <si>
-    <t>all types</t>
-  </si>
-  <si>
-    <t>What suggestions do you have?</t>
-  </si>
-  <si>
-    <t>more sleeping</t>
-  </si>
-  <si>
-    <t>RespondantInterested</t>
-  </si>
-  <si>
-    <t>Yes</t>
+    <t>Server:</t>
+  </si>
+  <si>
+    <t>DE-CODE-IT-001</t>
+  </si>
+  <si>
+    <t>IP:</t>
+  </si>
+  <si>
+    <t>68.229.180.106</t>
+  </si>
+  <si>
+    <t>Port:</t>
+  </si>
+  <si>
+    <t>FinalUser1</t>
+  </si>
+  <si>
+    <t>password1</t>
+  </si>
+  <si>
+    <t>Password:</t>
+  </si>
+  <si>
+    <t>UserName:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -324,10 +316,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -346,6 +344,55 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>376981</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>24829</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9928E88A-31B8-F4C3-A250-AF3E19D3B69C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2152650" y="57150"/>
+          <a:ext cx="6752381" cy="4571429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -707,148 +754,83 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BE5ED32-D4DC-46D4-B4E0-1A341603C793}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{885999FD-2B6E-4717-B138-0A9D8860C1F1}">
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="6.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="10.6328125" customWidth="1"/>
+    <col min="2" max="2" width="14.36328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" s="3">
+        <v>1433</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3142F5A-6D19-4460-8D8F-64E3C3F44186}">
-  <dimension ref="A1:O2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.26953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.90625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.7265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="31.7265625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="27.81640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.90625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="27.36328125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.54296875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I1" t="s">
-        <v>45</v>
-      </c>
-      <c r="J1" t="s">
-        <v>35</v>
-      </c>
-      <c r="K1" t="s">
-        <v>45</v>
-      </c>
-      <c r="L1" t="s">
-        <v>34</v>
-      </c>
-      <c r="M1" t="s">
-        <v>45</v>
-      </c>
-      <c r="N1" t="s">
-        <v>36</v>
-      </c>
-      <c r="O1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C2" t="s">
-        <v>65</v>
-      </c>
-      <c r="D2" t="s">
-        <v>66</v>
-      </c>
-      <c r="E2" t="s">
-        <v>67</v>
-      </c>
-      <c r="F2">
-        <v>83711</v>
-      </c>
-      <c r="G2" t="s">
-        <v>68</v>
-      </c>
-      <c r="H2" s="2">
-        <v>44984</v>
-      </c>
-      <c r="I2" t="s">
-        <v>69</v>
-      </c>
-      <c r="J2" t="s">
-        <v>70</v>
-      </c>
-      <c r="K2" t="s">
-        <v>71</v>
-      </c>
-      <c r="L2" t="s">
-        <v>72</v>
-      </c>
-      <c r="M2" t="s">
-        <v>73</v>
-      </c>
-      <c r="N2" t="s">
-        <v>74</v>
-      </c>
-      <c r="O2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{190D8C4D-480B-4471-B139-25F0F25963CB}">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView topLeftCell="B13" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView topLeftCell="B7" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
@@ -872,7 +854,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAEEC76D-4214-4C31-BA65-3A0F40B5FA47}">
   <dimension ref="A1:E9"/>
   <sheetViews>
@@ -1045,7 +1027,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4B139F5-5181-4C20-9F93-B5ABB35A51A1}">
   <dimension ref="A1:E13"/>
   <sheetViews>
@@ -1254,12 +1236,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81E89F66-4F82-4AED-AAE8-5E885C26EB89}">
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E8" sqref="A1:E8"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1421,7 +1403,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B881992B-9E09-4023-BB43-C01703BA0758}">
   <dimension ref="A1:E11"/>
   <sheetViews>
@@ -1585,7 +1567,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74CB8647-10B5-4C33-9795-076AD3A2B487}">
   <dimension ref="A1:E11"/>
   <sheetViews>

</xml_diff>